<commit_message>
update map to include multiple pins for multiple talks
</commit_message>
<xml_diff>
--- a/markdown_generator/all_talks.xlsx
+++ b/markdown_generator/all_talks.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>title</t>
   </si>
@@ -49,7 +49,7 @@
     <t>Special Session on Matrices and Graphs, AMS Central Section Meeting</t>
   </si>
   <si>
-    <t>Saint Paul, MN</t>
+    <t>St. Paul, MN</t>
   </si>
   <si>
     <t>Potentially eventually positive and potentially eventually exponentially positive sign patterns</t>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>MAA--North Central Sectional Meeting</t>
-  </si>
-  <si>
-    <t>St. Paul, MN</t>
   </si>
   <si>
     <t>Sign patterns that allow strong eventual nonnegativity</t>
@@ -812,7 +809,7 @@
         <v>39928.0</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -837,22 +834,22 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="3">
         <v>41118.0</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
@@ -877,22 +874,22 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" s="3">
         <v>41566.0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -917,16 +914,16 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E16" s="3">
         <v>40078.0</v>
@@ -957,16 +954,16 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E17" s="3">
         <v>40477.0</v>
@@ -997,16 +994,16 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="3">
         <v>40645.0</v>
@@ -1043,10 +1040,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" s="3">
         <v>40820.0</v>
@@ -1077,16 +1074,16 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="3">
         <v>41156.0</v>
@@ -1117,16 +1114,16 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21" s="3">
         <v>41240.0</v>
@@ -1163,10 +1160,10 @@
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E22" s="3">
         <v>41359.0</v>
@@ -1203,16 +1200,16 @@
         <v>9</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" s="3">
         <v>43389.0</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
@@ -1237,16 +1234,16 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E24" s="3">
         <v>40373.0</v>

</xml_diff>